<commit_message>
cuadro y cuaderno terminado casi
</commit_message>
<xml_diff>
--- a/Cuadro de noticias.xlsx
+++ b/Cuadro de noticias.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21126"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Documents\TESIS\Tesis\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF4B3428-7C70-4DE4-B0C2-460EA75D15D3}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -20,18 +21,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="999" uniqueCount="667">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1099" uniqueCount="735">
   <si>
     <t>DIARIO</t>
   </si>
@@ -1764,9 +1759,6 @@
     <t>La cámara de senadores intenta sancionar un proyecto de ley que penaliza con la cárcel a todos aquellos campesinos que enajenen sus derechos sobre el inmueble, es decir, sobre el lote otorgado por el estado.</t>
   </si>
   <si>
-    <t xml:space="preserve">En esta nota se realiza una fuerte crítica a todos aquellos legisladores que intentan sancionar esta ley, además se pone la atención sobre las autoridades del Indert y del IBR que no tienen ningún control sobre la cantidad de campesinos beneficiarios ni datos sobre ellos. En este caso, las críticas no son exclusivamente hacia la gestión de Lugo pero deja entrever que durante su gobierno poco se hixo en relación a la reforma agraria y a la situación de los campesinos.  </t>
-  </si>
-  <si>
     <t>Unasur - integración regional - Declaraciones</t>
   </si>
   <si>
@@ -2068,13 +2060,220 @@
   </si>
   <si>
     <t>Lo interesante en esta nota es que a partir del rechazo del congreso al veto presidencial, el diario asume y da por sentado que se transformará en un beneficio para Lugo ya que su mayor deseo, al igual que otros gobiernos latinoamericanos es terminar con las instituciones democráticas como el Parlamento. Al final se menciona "esta amenaza totalitaria! que Lugo vendría a encarnar que terminaría con la naciente democracia paraguaya. Finalmente se vuelve a mencionar el tema de las próximas elecciones y la manera en la que el pueblo paraguayo debería actuar.</t>
+  </si>
+  <si>
+    <t>Manifestación - Congreso - Proyecto de ley</t>
+  </si>
+  <si>
+    <t>El Congreso Nacional en peligro de muerte</t>
+  </si>
+  <si>
+    <t>La manifestación que se dio en frente del Congreso paraguayo en reclamo a la sanción que tuvo la ley que otorga una mayor partida presupuestaria para el Tribunal Electoral</t>
+  </si>
+  <si>
+    <t>Lo interesante en esta nota es que se vuelve a repetir la amenaza de Lugo sobre el Congreso y sobre la idea de terminar con el mismo. "la democracia representativa sufra una herida mortal de la que mucho se beneficiarán los que en el gobierno de Lugo abominan de ella, pretendiendo suplantarla por una nueva forma de autoritarismo".</t>
+  </si>
+  <si>
+    <t>Evo Morales - asilo político - senador opositor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Desde que la izquierda está en el poder, ya no se defiende a los perseguidos políticos </t>
+  </si>
+  <si>
+    <t>Sobre el pedido de asilo político del senador opositor al gobierno de Evo Morales que denunció a personas cercanas al presidente por estar relacionadas con el narcotráfico.</t>
+  </si>
+  <si>
+    <t>Siguiendo un tema recurrente el de "los presidentes que gobiernan bajo la férula del chavismo marxista bolivariano", vuelve a hacerse una crítica, en este caso, al gobierno boliviano mas precisamente a Evo Morales por las supuestas persecuciones políticas a opositores en su gobierno. Además se vuelve a mencionar la cuestión del Mercosur y Unasur como organismos que no tienen ningún tipo de injerencia en la política de los países.</t>
+  </si>
+  <si>
+    <t>Turistas VIP</t>
+  </si>
+  <si>
+    <t>Gira presidencial - Fernando Lugo - Representantes diplomáticos - Países asiáticos</t>
+  </si>
+  <si>
+    <t>Sobre los beneficios que podría traer consigo el presidente Fernando Lugo en su paso por los principales países asiáticos como Japón, Corea, Taiwán e India.</t>
+  </si>
+  <si>
+    <t>Editorial importante por el título, por el contenido y por el tono de la misma. Vuelve a plantear la idea de que los viajes de Lugo son puramente turísticos y que no representan ningún beneficio para el país. Además, utiliza recursos como preguntas retóricas, oraciones con signos de exclamación y afirmaciones sin ningún tipo de prueba.</t>
+  </si>
+  <si>
+    <t>Los líderes de la izquierda se olvidaron de los derechos humanos</t>
+  </si>
+  <si>
+    <t>Persecución política - derechos humanos - líderes de izquierda</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sobre la persecución política que supuestamente muchos gobiernos latinoamericanos están cometiendo contra periodistas y políticos opositores que hacen entender, que cometen los mismos delitos de los cuales ellos fueron víctimas en épocas dictatoriales. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vuelve a mencionarse el tema de la persecucion política en Latinoamérica y de la falta de solidaridad para con aquellos por parte de los presidentes latinoamericanos debido a su alianza ideológica. Tema muy recurrente en este diario. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pretender concretar el sueño dorado de los dictadores </t>
+  </si>
+  <si>
+    <t xml:space="preserve">CIDH - Derechos humanos - Unasur </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Los gobiernos de Venezuela, Ecuador y Bolivia anunciaron la creación de una instancia de Derechos Humanos en el marco de la UNASUR mientras que realizaron  fuertes críticas a la Comisión Interamericana de Derechos Humanos. </t>
+  </si>
+  <si>
+    <t>Nuevamente se vuelve  a mencionar el tema de los derechos humanos y los gobiernos "bolivarianos" de América Latina. En este caso se los nombra como: "un club de gobernantes autoritarios, enemigos de la libertad y violadores de los derechos humanos de los pueblos a los que miserablemente subyugan".</t>
+  </si>
+  <si>
+    <t>Denunciar a los infiltrados en las protestas ciudadanas</t>
+  </si>
+  <si>
+    <t>Manifestaciones ciudadanas - actos vandálicos - partidos políticos</t>
+  </si>
+  <si>
+    <t>Los actos de violencia y vandalismo que sufrieron las instalaciones de los dos partidos políticos tradicionales de Paraguay durante las manifestaciones que tuvieron lugar en Asunción con el fin de rechazar la postergacion de la ley que terminaría con las listas sábanas.</t>
+  </si>
+  <si>
+    <t>Lo interesante en esta editorial es cómo a partir de actos de violencia que desataron un grupo de personas que aun no fueron identificados, se asocia que podrían responder al gobierno de Lugo en función de generar crisis internas al interior de los partidos políticos tradicionales. Todas muestras de "futurismo", predicciones, vaticinios casi trágicos para la democracia paraguay. Por ejemplo:"podrían constituir el ariete de un eficiente intento por restaurar una dictadura en nuestro país, aunque no precisamente de derecha".</t>
+  </si>
+  <si>
+    <t>Asamblea General de la OEA - Jorge Lara Castro - Declaraciones</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Le echan la culpa a otros de su inutilidad </t>
+  </si>
+  <si>
+    <t>Las declaraciones realizadas por el Canciller Jorge Lara Castro en la Asamblea General de la Oea sobre el diagnóstico económico en Paraguay, particularmente con la situación del campo.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Esta nota vuelve a referir a lo no realizado por el gobierno de Fernando Lugo en términos de reforma agraria y mejoras en las condiciones de vida de los campesinos. Vuelve a mencionar la idea del gobierno "del cambio" y vuelve a plantear que sus funcionarios desconocen la realidad económica paraguaya y son incapaces de encontrar soluciones al problema del campo. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">La incoherencia a ritmo de samba </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ministro secretario del Ambiente - Cumbre sobre Desarrollo Sostenible </t>
+  </si>
+  <si>
+    <t>Vuelve a mencionarse la incoherencia en el gobierno de Lugo entre lo que dice y cómo actúa. (enumera una serie de incoherencias en la nota). Además vuelve a jugar con la idea "del gobierno del cambio" que se repite numerosas veces en la editorial. Además vuelve a plantear que se mantuvieron ciertas caracteristicas existentes en los gobiernos colorados anteriores y que la gestión de Lugo tuvo "las más perversas prácticas de amiguismo, clientela política y manejos poco claros se mantienen rampantes en las instituciones públicas. Se cumplió como nunca aquello de “que cambie todo, para que no cambie absolutamente nada”.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El Ministro Secretario del Ambiente se trasladará con un grupo a la Cumbre de Desarrollo Sostenible Río+20 y esto generó numerosas críticas del diario. </t>
+  </si>
+  <si>
+    <t>Compromiso petrolero - PDVSA - deuda millonaria</t>
+  </si>
+  <si>
+    <t>¿Quién le robó los US$ 290 millones a Petropar?</t>
+  </si>
+  <si>
+    <t>El presidente de Petropar, Sergio Escobar, propone que PDVSA goce por seis meses de un monopolio de la venta del gasoíl, para pagar “la maldita deuda de PDVSA".</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nuevamente se menciona la influencia de Chavez en la región, en este caso, a partir de la negociación del petróleo. A pesar de que la deuda contraida con PDVSA se inció en el gobierno de Nicanor Duarte Frutos, el diario no deja de resaltar que se multiplicó durante "el gobierno del cambio". Interesante por el tono de la editorial y por la apelación a preguntas retóricas y como en casi todas las editoriales, a exhortar a la ciudadanía a actuar frente a "estos atropellos" que sufren los ciudadanos. </t>
+  </si>
+  <si>
+    <t>Democracia “flexible” a la medida…</t>
+  </si>
+  <si>
+    <t>Democracia "flexible" - democracia representativa - gobiernos bolivarianos</t>
+  </si>
+  <si>
+    <t>La definición de democracias "flexibles" por parte de la ex secretaria general de la Unasur para hablar de los países latinoamericanos, abre una serie de críticas en el diario sobre los gobiernos bolivarianos y el peligro de la democracia representativa.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nuevamente el tema en discusión responde a los llamados "gobiernos bolivarianos". En este caso, los define como: "los exponentes de ese engendro conocido como “bolivarianismo socialista del siglo XXI”, nuevo nombre para el fracasado marxismo, enemigo de la libertad y la propiedad privada". Tema muy recurrente para el diario en sus notas editoriales. </t>
+  </si>
+  <si>
+    <t>El presidente Lugo es el responsable de esta lamentable tragedia</t>
+  </si>
+  <si>
+    <t>Violencia - Curuguaty - grupos radicalizados</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Los graves incidentes sucedidos en Curuguaty que dejó el saldo de 15 personas muertas entre policías y manifestantes, pone al presidente Lugo en la mira de las acusaciones. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Editorial en la cual se trata el incidente de Curuguaty. A diferencia del diario Ultima Hora, en este, el presidente Lugo se nombra como el principal responsable de la masacre. Se menciona directamente su relación con estos grupos radicalizados y su incompetencia a la hora de resolver el problema de los campesinos. Incluso se nombra de manera directa la posibilidad de llevarlo a juicio político : "el presidente Lugo tal vez vuelva a eludir –más producto de la suerte que de cualquier otra circunstancia– la posibilidad de ser sometido a un proceso político en el Congreso que derive en su eventual remoción del cargo. Es probable que tenga esa suerte". </t>
+  </si>
+  <si>
+    <t>Responsabilidad inexcusable</t>
+  </si>
+  <si>
+    <t>Curuguaty - EPP - Gobierno de Fernando Lugo</t>
+  </si>
+  <si>
+    <t>Las responsabilidades que le competen al gobierno de Fernando Lugo por lo acontecido en Curuguaty y su supuesto acercamiento al grupo denominado EPP.</t>
+  </si>
+  <si>
+    <t>En esta editorial vuleve a tratarse el tema de Curuguaty y la responsabilidad de Lugo en el hecho. Se menciona nuevamente su cercanìa con el grupo EPP y sus desatenciones a las normativas jurídicas sobre la propiedad privada. En esta nota, el diario hace una declaracón concreta de pedido de juicio político al presidente: "Si en esta oportunidad el Poder Ejecutivo no actúa enérgicamente contra los grupos criminales y violentos que mantienen en zozobra a todo el país, el Congreso debería iniciarle juicio político al Presidente de la República por mal desempeño de funciones".</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Curuguaty - respuestas - crisis política </t>
+  </si>
+  <si>
+    <t xml:space="preserve">¿Quiénes y para qué? </t>
+  </si>
+  <si>
+    <t>La necesidad de obtener respuestas frente a lo sucedido en Curuguaty que abre un panorama de crisis política en Paraguay.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">En este caso, la editorial plantea una serie de interrogantes que considera deben ser respondidos. Para el diario el EPP es el principal responsable de la masacre, por ende, el gobierno de Lugo por su cercanía y afinidad, tiene relación en el hecho. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">País a la deriva </t>
+  </si>
+  <si>
+    <t>Declaraciones - Obispo de Caacupé - Conducción - Fernando Lugo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sobre las declaraciones emitidas por el obispo de Caacupé en relación a lo sucedido en Cuaruguaty y la falta de conducción del presidente Fernando Lugo. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Otra editorial que dice claramente que la responsabilidad de lo acontecido recae sobre el presidente Fernando Lugo. Vuelve a mencionar sus promesas de campaña incumplidas, y plantea que hay una "ausencia de un necesario liderazgo político", "Fernando Lugo no tiene el “don de conducción”. Utiliza recursos como preguntas retóricas que luego se responden a sí mismos, además de citar frases que el presidente habia dicho en su momento. </t>
+  </si>
+  <si>
+    <t>Fernando Lugo - Juicio Político - Líderes bolivarianos</t>
+  </si>
+  <si>
+    <t>Una comisión para el “oparei"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">De qué manera debería actuar el presidente Fernando Lugo, luego de haber transcurrido una semana desde el suceso de Curuguaty y la manera en la que los líderes bolivarianos actuarían ante un posible juicio político. </t>
+  </si>
+  <si>
+    <t>Esta editorial resulta interesante ya que plantea cómo actuarían los presidentes latinoamericanos frente a un posible juicio político a Fernando Lugo, teniendo en cuenta que en el día de la nota aún el proceso de destitución aún no había empezado. El diario ya lo daba por hecho y casi como que intentaba justificar el proceso antes de comenzar. Se vuelve a mencionar el tema del Protocolo de Ushuaia y de Unasur. También se expresa claramente: "Quien debió someterse espontánea e inmediatamente a un juicio político tuvo que haber sido el actual Presidente de la República, primer responsable de estos sucesos".</t>
+  </si>
+  <si>
+    <t>Lugo perdió el respaldo de la mayoría del pueblo paraguayo</t>
+  </si>
+  <si>
+    <t>Juicio Político - Fernando Lugo - Apoyo social</t>
+  </si>
+  <si>
+    <t>La nota plantea que Lugo al haberse quedado sin el apoyo del PLRA, no cuenta con el apoyo social con el cual inició su mandato presidencial a la hora de enfrentar el proceso de juicio político.</t>
+  </si>
+  <si>
+    <t>Esta nota refiere al día de la destitución de Lugo finalmente. Lo interesante es que el diario afirma que Lugo se quedó sin el apoyo social por el simple hecho de que no cuenta con el apoyo del PLRA y de la mayoría de los partidos políticos en el Congreso. Además plantea ciertos números, como por ejemplo: "El Partido Liberal Radical Auténtico (PLRA), miembro principal de la Alianza Patriótica para el Cambio que lo aupó al poder, le aportó 507.000 votos, es decir, el 66% del total". Interesante por el título, el contenido y el tono de la nota en donde en vez de una editorial crítica apela a cuestiones como la esperanza, que se vaya por la puerta grande, sensatez, grandeza de espíritu....</t>
+  </si>
+  <si>
+    <t>Otra etapa con nuevas esperanzas</t>
+  </si>
+  <si>
+    <t>Destitución presidencial - Federico Franco - ciudadanía</t>
+  </si>
+  <si>
+    <t>Finalmente, se dio la destitución de Fernando Lugo y la llegada a la presidencia de su vice Federico Franco frente a una ciudadanía que no realizó ningún tipo de manifestación importante en rechazo al proceso político.</t>
+  </si>
+  <si>
+    <t>Esta nota casi que agradece a la clase política el proceso realizado, además que considera que la actitud de la ciudadanía estuvo a la altura y no "ensombrecieron el paisaje democrático en estos días" como si el proceso como se dió lo haya sido. Para el diario, claramente se dieron las condiciones democráticas en este caso y la velocidad del mismo fue correcto. Resulta interesante leer el último parrafo de la nota que dice:  "ABC Color desea al presidente Federico Franco el mayor de los éxitos en su misión, en bien de todos, como en su momento también se deseó lo mismo, con la mayor sinceridad, al expresidente Lugo. De su gestión depende la recuperación del optimismo y la esperanza de que esta etapa política, la que hoy se inicia, sea tan luminosa como la que todo el pueblo paraguayo anhela"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">En esta nota se realiza una fuerte crítica a todos aquellos legisladores que intentan sancionar esta ley, además se pone la atención sobre las autoridades del Indert y del IBR que no tienen ningún control sobre la cantidad de campesinos beneficiarios ni datos sobre ellos. En este caso, las críticas no son exclusivamente hacia la gestión de Lugo pero deja entrever que durante su gobierno poco se hizo en relación a la reforma agraria y a la situación de los campesinos.  </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2115,6 +2314,12 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -2172,7 +2377,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2213,6 +2418,12 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2493,11 +2704,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:G172"/>
   <sheetViews>
-    <sheetView topLeftCell="A135" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView topLeftCell="A120" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2530,7 +2741,7 @@
         <v>5</v>
       </c>
       <c r="G2" s="16" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -5986,11 +6197,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:G65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6024,10 +6235,10 @@
         <v>5</v>
       </c>
       <c r="G1" s="15" t="s">
-        <v>626</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" ht="132.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>625</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="104.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>556</v>
       </c>
@@ -6050,7 +6261,7 @@
         <v>561</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="152.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" ht="118.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>556</v>
       </c>
@@ -6070,15 +6281,15 @@
         <v>564</v>
       </c>
       <c r="G3" s="8" t="s">
-        <v>565</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" ht="204.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>734</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="168.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>556</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="C4" s="6">
         <v>40992</v>
@@ -6087,13 +6298,13 @@
         <v>558</v>
       </c>
       <c r="E4" s="8" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="F4" s="8" t="s">
+        <v>567</v>
+      </c>
+      <c r="G4" s="8" t="s">
         <v>568</v>
-      </c>
-      <c r="G4" s="8" t="s">
-        <v>569</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="153" customHeight="1" x14ac:dyDescent="0.25">
@@ -6101,7 +6312,7 @@
         <v>556</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="C5" s="6">
         <v>40993</v>
@@ -6110,21 +6321,21 @@
         <v>558</v>
       </c>
       <c r="E5" s="8" t="s">
+        <v>570</v>
+      </c>
+      <c r="F5" s="8" t="s">
         <v>571</v>
       </c>
-      <c r="F5" s="8" t="s">
+      <c r="G5" s="8" t="s">
         <v>572</v>
       </c>
-      <c r="G5" s="8" t="s">
-        <v>573</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" ht="128.25" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:7" ht="108" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>556</v>
       </c>
-      <c r="B6" s="4" t="s">
-        <v>574</v>
+      <c r="B6" s="8" t="s">
+        <v>573</v>
       </c>
       <c r="C6" s="6">
         <v>40996</v>
@@ -6133,13 +6344,13 @@
         <v>558</v>
       </c>
       <c r="E6" s="8" t="s">
+        <v>574</v>
+      </c>
+      <c r="F6" s="8" t="s">
         <v>575</v>
       </c>
-      <c r="F6" s="8" t="s">
+      <c r="G6" s="8" t="s">
         <v>576</v>
-      </c>
-      <c r="G6" s="8" t="s">
-        <v>577</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="142.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -6147,7 +6358,7 @@
         <v>556</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="C7" s="6">
         <v>40998</v>
@@ -6156,13 +6367,13 @@
         <v>558</v>
       </c>
       <c r="E7" s="8" t="s">
+        <v>578</v>
+      </c>
+      <c r="F7" s="8" t="s">
         <v>579</v>
       </c>
-      <c r="F7" s="8" t="s">
+      <c r="G7" s="8" t="s">
         <v>580</v>
-      </c>
-      <c r="G7" s="8" t="s">
-        <v>581</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="181.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -6170,7 +6381,7 @@
         <v>556</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="C8" s="6">
         <v>41000</v>
@@ -6179,13 +6390,13 @@
         <v>558</v>
       </c>
       <c r="E8" s="8" t="s">
+        <v>582</v>
+      </c>
+      <c r="F8" s="8" t="s">
         <v>583</v>
       </c>
-      <c r="F8" s="8" t="s">
+      <c r="G8" s="8" t="s">
         <v>584</v>
-      </c>
-      <c r="G8" s="8" t="s">
-        <v>585</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="129" customHeight="1" x14ac:dyDescent="0.25">
@@ -6193,7 +6404,7 @@
         <v>556</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="C9" s="6">
         <v>41001</v>
@@ -6202,13 +6413,13 @@
         <v>558</v>
       </c>
       <c r="E9" s="8" t="s">
+        <v>586</v>
+      </c>
+      <c r="F9" s="8" t="s">
         <v>587</v>
       </c>
-      <c r="F9" s="8" t="s">
+      <c r="G9" s="8" t="s">
         <v>588</v>
-      </c>
-      <c r="G9" s="8" t="s">
-        <v>589</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="154.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -6216,7 +6427,7 @@
         <v>556</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="C10" s="6">
         <v>41002</v>
@@ -6225,13 +6436,13 @@
         <v>558</v>
       </c>
       <c r="E10" s="8" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="F10" s="8" t="s">
+        <v>591</v>
+      </c>
+      <c r="G10" s="8" t="s">
         <v>592</v>
-      </c>
-      <c r="G10" s="8" t="s">
-        <v>593</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="207" customHeight="1" x14ac:dyDescent="0.25">
@@ -6239,7 +6450,7 @@
         <v>556</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="C11" s="6">
         <v>41004</v>
@@ -6248,13 +6459,13 @@
         <v>558</v>
       </c>
       <c r="E11" s="8" t="s">
+        <v>594</v>
+      </c>
+      <c r="F11" s="8" t="s">
         <v>595</v>
       </c>
-      <c r="F11" s="8" t="s">
+      <c r="G11" s="8" t="s">
         <v>596</v>
-      </c>
-      <c r="G11" s="8" t="s">
-        <v>597</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="115.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -6262,7 +6473,7 @@
         <v>556</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="C12" s="6">
         <v>41007</v>
@@ -6271,13 +6482,13 @@
         <v>558</v>
       </c>
       <c r="E12" s="8" t="s">
+        <v>598</v>
+      </c>
+      <c r="F12" s="8" t="s">
         <v>599</v>
       </c>
-      <c r="F12" s="8" t="s">
+      <c r="G12" s="8" t="s">
         <v>600</v>
-      </c>
-      <c r="G12" s="8" t="s">
-        <v>601</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="78" customHeight="1" x14ac:dyDescent="0.25">
@@ -6285,7 +6496,7 @@
         <v>556</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="C13" s="6">
         <v>41009</v>
@@ -6294,13 +6505,13 @@
         <v>558</v>
       </c>
       <c r="E13" s="8" t="s">
+        <v>603</v>
+      </c>
+      <c r="F13" s="8" t="s">
+        <v>602</v>
+      </c>
+      <c r="G13" s="8" t="s">
         <v>604</v>
-      </c>
-      <c r="F13" s="8" t="s">
-        <v>603</v>
-      </c>
-      <c r="G13" s="8" t="s">
-        <v>605</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="81" customHeight="1" x14ac:dyDescent="0.25">
@@ -6308,7 +6519,7 @@
         <v>556</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="C14" s="6">
         <v>41011</v>
@@ -6317,13 +6528,13 @@
         <v>558</v>
       </c>
       <c r="E14" s="8" t="s">
+        <v>606</v>
+      </c>
+      <c r="F14" s="8" t="s">
         <v>607</v>
       </c>
-      <c r="F14" s="8" t="s">
+      <c r="G14" s="8" t="s">
         <v>608</v>
-      </c>
-      <c r="G14" s="8" t="s">
-        <v>609</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="129.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -6331,7 +6542,7 @@
         <v>556</v>
       </c>
       <c r="B15" s="8" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="C15" s="6">
         <v>41012</v>
@@ -6340,13 +6551,13 @@
         <v>558</v>
       </c>
       <c r="E15" s="8" t="s">
+        <v>610</v>
+      </c>
+      <c r="F15" s="8" t="s">
         <v>611</v>
       </c>
-      <c r="F15" s="8" t="s">
+      <c r="G15" s="8" t="s">
         <v>612</v>
-      </c>
-      <c r="G15" s="8" t="s">
-        <v>613</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="168.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -6354,7 +6565,7 @@
         <v>556</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="C16" s="6">
         <v>41013</v>
@@ -6363,21 +6574,21 @@
         <v>558</v>
       </c>
       <c r="E16" s="8" t="s">
+        <v>614</v>
+      </c>
+      <c r="F16" s="8" t="s">
         <v>615</v>
       </c>
-      <c r="F16" s="8" t="s">
+      <c r="G16" s="8" t="s">
         <v>616</v>
       </c>
-      <c r="G16" s="8" t="s">
-        <v>617</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" ht="142.5" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="1:7" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
         <v>556</v>
       </c>
       <c r="B17" s="8" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="C17" s="6">
         <v>41014</v>
@@ -6386,21 +6597,21 @@
         <v>558</v>
       </c>
       <c r="E17" s="8" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="F17" s="8" t="s">
+        <v>619</v>
+      </c>
+      <c r="G17" s="8" t="s">
         <v>620</v>
       </c>
-      <c r="G17" s="8" t="s">
-        <v>621</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" ht="144" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="1:7" ht="119.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
         <v>556</v>
       </c>
       <c r="B18" s="8" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="C18" s="6">
         <v>41018</v>
@@ -6409,13 +6620,13 @@
         <v>558</v>
       </c>
       <c r="E18" s="8" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="F18" s="8" t="s">
+        <v>623</v>
+      </c>
+      <c r="G18" s="8" t="s">
         <v>624</v>
-      </c>
-      <c r="G18" s="8" t="s">
-        <v>625</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -6423,7 +6634,7 @@
         <v>556</v>
       </c>
       <c r="B19" s="8" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="C19" s="6">
         <v>41020</v>
@@ -6432,13 +6643,13 @@
         <v>558</v>
       </c>
       <c r="E19" s="8" t="s">
+        <v>627</v>
+      </c>
+      <c r="F19" s="8" t="s">
         <v>628</v>
       </c>
-      <c r="F19" s="8" t="s">
+      <c r="G19" s="8" t="s">
         <v>629</v>
-      </c>
-      <c r="G19" s="8" t="s">
-        <v>630</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="115.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -6446,7 +6657,7 @@
         <v>556</v>
       </c>
       <c r="B20" s="8" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="C20" s="6">
         <v>41028</v>
@@ -6455,13 +6666,13 @@
         <v>558</v>
       </c>
       <c r="E20" s="8" t="s">
+        <v>631</v>
+      </c>
+      <c r="F20" s="8" t="s">
         <v>632</v>
       </c>
-      <c r="F20" s="8" t="s">
+      <c r="G20" s="8" t="s">
         <v>633</v>
-      </c>
-      <c r="G20" s="8" t="s">
-        <v>634</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="132" customHeight="1" x14ac:dyDescent="0.25">
@@ -6469,7 +6680,7 @@
         <v>556</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="C21" s="6">
         <v>41032</v>
@@ -6478,13 +6689,13 @@
         <v>558</v>
       </c>
       <c r="E21" s="8" t="s">
+        <v>635</v>
+      </c>
+      <c r="F21" s="8" t="s">
         <v>636</v>
       </c>
-      <c r="F21" s="8" t="s">
+      <c r="G21" s="8" t="s">
         <v>637</v>
-      </c>
-      <c r="G21" s="8" t="s">
-        <v>638</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="115.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -6492,7 +6703,7 @@
         <v>556</v>
       </c>
       <c r="B22" s="8" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
       <c r="C22" s="6">
         <v>41038</v>
@@ -6501,13 +6712,13 @@
         <v>558</v>
       </c>
       <c r="E22" s="8" t="s">
+        <v>639</v>
+      </c>
+      <c r="F22" s="8" t="s">
         <v>640</v>
       </c>
-      <c r="F22" s="8" t="s">
+      <c r="G22" s="8" t="s">
         <v>641</v>
-      </c>
-      <c r="G22" s="8" t="s">
-        <v>642</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="157.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -6515,7 +6726,7 @@
         <v>556</v>
       </c>
       <c r="B23" s="8" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="C23" s="6">
         <v>41040</v>
@@ -6524,13 +6735,13 @@
         <v>558</v>
       </c>
       <c r="E23" s="8" t="s">
+        <v>643</v>
+      </c>
+      <c r="F23" s="8" t="s">
         <v>644</v>
       </c>
-      <c r="F23" s="8" t="s">
+      <c r="G23" s="8" t="s">
         <v>645</v>
-      </c>
-      <c r="G23" s="8" t="s">
-        <v>646</v>
       </c>
     </row>
     <row r="24" spans="1:7" ht="117" customHeight="1" x14ac:dyDescent="0.25">
@@ -6538,7 +6749,7 @@
         <v>556</v>
       </c>
       <c r="B24" s="8" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="C24" s="6">
         <v>41042</v>
@@ -6547,13 +6758,13 @@
         <v>558</v>
       </c>
       <c r="E24" s="8" t="s">
+        <v>647</v>
+      </c>
+      <c r="F24" s="8" t="s">
         <v>648</v>
       </c>
-      <c r="F24" s="8" t="s">
+      <c r="G24" s="8" t="s">
         <v>649</v>
-      </c>
-      <c r="G24" s="8" t="s">
-        <v>650</v>
       </c>
     </row>
     <row r="25" spans="1:7" ht="117" customHeight="1" x14ac:dyDescent="0.25">
@@ -6561,7 +6772,7 @@
         <v>556</v>
       </c>
       <c r="B25" s="8" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
       <c r="C25" s="6">
         <v>41046</v>
@@ -6570,13 +6781,13 @@
         <v>558</v>
       </c>
       <c r="E25" s="8" t="s">
+        <v>651</v>
+      </c>
+      <c r="F25" s="8" t="s">
         <v>652</v>
       </c>
-      <c r="F25" s="8" t="s">
+      <c r="G25" s="8" t="s">
         <v>653</v>
-      </c>
-      <c r="G25" s="8" t="s">
-        <v>654</v>
       </c>
     </row>
     <row r="26" spans="1:7" ht="66.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -6584,7 +6795,7 @@
         <v>556</v>
       </c>
       <c r="B26" s="8" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
       <c r="C26" s="6">
         <v>41048</v>
@@ -6593,13 +6804,13 @@
         <v>558</v>
       </c>
       <c r="E26" s="8" t="s">
+        <v>655</v>
+      </c>
+      <c r="F26" s="8" t="s">
         <v>656</v>
       </c>
-      <c r="F26" s="8" t="s">
+      <c r="G26" s="8" t="s">
         <v>657</v>
-      </c>
-      <c r="G26" s="8" t="s">
-        <v>658</v>
       </c>
     </row>
     <row r="27" spans="1:7" ht="180" customHeight="1" x14ac:dyDescent="0.25">
@@ -6607,7 +6818,7 @@
         <v>556</v>
       </c>
       <c r="B27" s="8" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="C27" s="6">
         <v>41049</v>
@@ -6616,13 +6827,13 @@
         <v>558</v>
       </c>
       <c r="E27" s="8" t="s">
+        <v>659</v>
+      </c>
+      <c r="F27" s="8" t="s">
         <v>660</v>
       </c>
-      <c r="F27" s="8" t="s">
+      <c r="G27" s="8" t="s">
         <v>661</v>
-      </c>
-      <c r="G27" s="8" t="s">
-        <v>662</v>
       </c>
     </row>
     <row r="28" spans="1:7" ht="143.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -6630,7 +6841,7 @@
         <v>556</v>
       </c>
       <c r="B28" s="8" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="C28" s="6">
         <v>41054</v>
@@ -6639,234 +6850,468 @@
         <v>558</v>
       </c>
       <c r="E28" s="8" t="s">
+        <v>663</v>
+      </c>
+      <c r="F28" s="8" t="s">
         <v>664</v>
       </c>
-      <c r="F28" s="8" t="s">
+      <c r="G28" s="8" t="s">
         <v>665</v>
       </c>
-      <c r="G28" s="8" t="s">
-        <v>666</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="29" spans="1:7" ht="90" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
         <v>556</v>
       </c>
-      <c r="B29" s="4"/>
-      <c r="C29" s="4"/>
+      <c r="B29" s="8" t="s">
+        <v>667</v>
+      </c>
+      <c r="C29" s="6">
+        <v>41056</v>
+      </c>
       <c r="D29" s="4" t="s">
         <v>558</v>
       </c>
-      <c r="E29" s="4"/>
-      <c r="F29" s="4"/>
-      <c r="G29" s="4"/>
-    </row>
-    <row r="30" spans="1:7" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="4"/>
-      <c r="B30" s="4"/>
-      <c r="C30" s="4"/>
-      <c r="D30" s="4"/>
-      <c r="E30" s="4"/>
-      <c r="F30" s="4"/>
-      <c r="G30" s="4"/>
-    </row>
-    <row r="31" spans="1:7" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="4"/>
-      <c r="B31" s="4"/>
-      <c r="C31" s="4"/>
-      <c r="D31" s="4"/>
-      <c r="E31" s="4"/>
-      <c r="F31" s="4"/>
-      <c r="G31" s="4"/>
-    </row>
-    <row r="32" spans="1:7" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="4"/>
-      <c r="B32" s="4"/>
-      <c r="C32" s="4"/>
-      <c r="D32" s="4"/>
-      <c r="E32" s="4"/>
-      <c r="F32" s="4"/>
-      <c r="G32" s="4"/>
-    </row>
-    <row r="33" spans="1:7" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="4"/>
-      <c r="B33" s="4"/>
-      <c r="C33" s="4"/>
-      <c r="D33" s="4"/>
-      <c r="E33" s="4"/>
-      <c r="F33" s="4"/>
-      <c r="G33" s="4"/>
-    </row>
-    <row r="34" spans="1:7" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="4"/>
-      <c r="B34" s="4"/>
-      <c r="C34" s="4"/>
-      <c r="D34" s="4"/>
-      <c r="E34" s="4"/>
-      <c r="F34" s="4"/>
-      <c r="G34" s="4"/>
-    </row>
-    <row r="35" spans="1:7" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="4"/>
-      <c r="B35" s="4"/>
-      <c r="C35" s="4"/>
-      <c r="D35" s="4"/>
-      <c r="E35" s="4"/>
-      <c r="F35" s="4"/>
-      <c r="G35" s="4"/>
-    </row>
-    <row r="36" spans="1:7" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="4"/>
-      <c r="B36" s="4"/>
-      <c r="C36" s="4"/>
-      <c r="D36" s="4"/>
-      <c r="E36" s="4"/>
-      <c r="F36" s="4"/>
-      <c r="G36" s="4"/>
-    </row>
-    <row r="37" spans="1:7" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="1"/>
-      <c r="B37" s="1"/>
-      <c r="C37" s="1"/>
-      <c r="D37" s="1"/>
-      <c r="E37" s="1"/>
-      <c r="F37" s="1"/>
-      <c r="G37" s="1"/>
-    </row>
-    <row r="38" spans="1:7" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="1"/>
-      <c r="B38" s="1"/>
-      <c r="C38" s="1"/>
-      <c r="D38" s="1"/>
-      <c r="E38" s="1"/>
-      <c r="F38" s="1"/>
-      <c r="G38" s="1"/>
-    </row>
-    <row r="39" spans="1:7" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="1"/>
-      <c r="B39" s="1"/>
-      <c r="C39" s="1"/>
-      <c r="D39" s="1"/>
-      <c r="E39" s="1"/>
-      <c r="F39" s="1"/>
-      <c r="G39" s="1"/>
-    </row>
-    <row r="40" spans="1:7" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="1"/>
-      <c r="B40" s="1"/>
-      <c r="C40" s="1"/>
-      <c r="D40" s="1"/>
-      <c r="E40" s="1"/>
-      <c r="F40" s="1"/>
-      <c r="G40" s="1"/>
-    </row>
-    <row r="41" spans="1:7" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="1"/>
-      <c r="B41" s="1"/>
-      <c r="C41" s="1"/>
-      <c r="D41" s="1"/>
-      <c r="E41" s="1"/>
-      <c r="F41" s="1"/>
-      <c r="G41" s="1"/>
-    </row>
-    <row r="42" spans="1:7" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="1"/>
-      <c r="B42" s="1"/>
-      <c r="C42" s="1"/>
-      <c r="D42" s="1"/>
-      <c r="E42" s="1"/>
-      <c r="F42" s="1"/>
-      <c r="G42" s="1"/>
-    </row>
-    <row r="43" spans="1:7" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="1"/>
-      <c r="B43" s="1"/>
-      <c r="C43" s="1"/>
-      <c r="D43" s="1"/>
-      <c r="E43" s="1"/>
-      <c r="F43" s="1"/>
-      <c r="G43" s="1"/>
-    </row>
-    <row r="44" spans="1:7" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="1"/>
-      <c r="B44" s="1"/>
-      <c r="C44" s="1"/>
-      <c r="D44" s="1"/>
-      <c r="E44" s="1"/>
-      <c r="F44" s="1"/>
-      <c r="G44" s="1"/>
-    </row>
-    <row r="45" spans="1:7" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="1"/>
-      <c r="B45" s="1"/>
-      <c r="C45" s="1"/>
-      <c r="D45" s="1"/>
-      <c r="E45" s="1"/>
-      <c r="F45" s="1"/>
-      <c r="G45" s="1"/>
+      <c r="E29" s="8" t="s">
+        <v>666</v>
+      </c>
+      <c r="F29" s="8" t="s">
+        <v>668</v>
+      </c>
+      <c r="G29" s="8" t="s">
+        <v>669</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" ht="116.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="4" t="s">
+        <v>556</v>
+      </c>
+      <c r="B30" s="8" t="s">
+        <v>671</v>
+      </c>
+      <c r="C30" s="6">
+        <v>41060</v>
+      </c>
+      <c r="D30" s="4" t="s">
+        <v>558</v>
+      </c>
+      <c r="E30" s="8" t="s">
+        <v>670</v>
+      </c>
+      <c r="F30" s="8" t="s">
+        <v>672</v>
+      </c>
+      <c r="G30" s="8" t="s">
+        <v>673</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" ht="91.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="4" t="s">
+        <v>556</v>
+      </c>
+      <c r="B31" s="4" t="s">
+        <v>674</v>
+      </c>
+      <c r="C31" s="6">
+        <v>41061</v>
+      </c>
+      <c r="D31" s="4" t="s">
+        <v>558</v>
+      </c>
+      <c r="E31" s="8" t="s">
+        <v>675</v>
+      </c>
+      <c r="F31" s="8" t="s">
+        <v>676</v>
+      </c>
+      <c r="G31" s="8" t="s">
+        <v>677</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" ht="67.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="4" t="s">
+        <v>556</v>
+      </c>
+      <c r="B32" s="8" t="s">
+        <v>678</v>
+      </c>
+      <c r="C32" s="6">
+        <v>41063</v>
+      </c>
+      <c r="D32" s="4" t="s">
+        <v>558</v>
+      </c>
+      <c r="E32" s="8" t="s">
+        <v>679</v>
+      </c>
+      <c r="F32" s="8" t="s">
+        <v>680</v>
+      </c>
+      <c r="G32" s="8" t="s">
+        <v>681</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" ht="78.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="4" t="s">
+        <v>556</v>
+      </c>
+      <c r="B33" s="8" t="s">
+        <v>682</v>
+      </c>
+      <c r="C33" s="6">
+        <v>41066</v>
+      </c>
+      <c r="D33" s="4" t="s">
+        <v>558</v>
+      </c>
+      <c r="E33" s="8" t="s">
+        <v>683</v>
+      </c>
+      <c r="F33" s="8" t="s">
+        <v>684</v>
+      </c>
+      <c r="G33" s="8" t="s">
+        <v>685</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" ht="142.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="4" t="s">
+        <v>556</v>
+      </c>
+      <c r="B34" s="14" t="s">
+        <v>686</v>
+      </c>
+      <c r="C34" s="6">
+        <v>41068</v>
+      </c>
+      <c r="D34" s="4" t="s">
+        <v>558</v>
+      </c>
+      <c r="E34" s="8" t="s">
+        <v>687</v>
+      </c>
+      <c r="F34" s="8" t="s">
+        <v>688</v>
+      </c>
+      <c r="G34" s="8" t="s">
+        <v>689</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" ht="105.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="4" t="s">
+        <v>556</v>
+      </c>
+      <c r="B35" s="8" t="s">
+        <v>691</v>
+      </c>
+      <c r="C35" s="6">
+        <v>41069</v>
+      </c>
+      <c r="D35" s="4" t="s">
+        <v>558</v>
+      </c>
+      <c r="E35" s="8" t="s">
+        <v>690</v>
+      </c>
+      <c r="F35" s="8" t="s">
+        <v>692</v>
+      </c>
+      <c r="G35" s="8" t="s">
+        <v>693</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" ht="154.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="4" t="s">
+        <v>556</v>
+      </c>
+      <c r="B36" s="8" t="s">
+        <v>694</v>
+      </c>
+      <c r="C36" s="6">
+        <v>41070</v>
+      </c>
+      <c r="D36" s="4" t="s">
+        <v>558</v>
+      </c>
+      <c r="E36" s="8" t="s">
+        <v>695</v>
+      </c>
+      <c r="F36" s="8" t="s">
+        <v>697</v>
+      </c>
+      <c r="G36" s="17" t="s">
+        <v>696</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" ht="130.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="4" t="s">
+        <v>556</v>
+      </c>
+      <c r="B37" s="8" t="s">
+        <v>699</v>
+      </c>
+      <c r="C37" s="6">
+        <v>41073</v>
+      </c>
+      <c r="D37" s="4" t="s">
+        <v>558</v>
+      </c>
+      <c r="E37" s="8" t="s">
+        <v>698</v>
+      </c>
+      <c r="F37" s="8" t="s">
+        <v>700</v>
+      </c>
+      <c r="G37" s="8" t="s">
+        <v>701</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" ht="93" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="4" t="s">
+        <v>556</v>
+      </c>
+      <c r="B38" s="8" t="s">
+        <v>702</v>
+      </c>
+      <c r="C38" s="6">
+        <v>41075</v>
+      </c>
+      <c r="D38" s="4" t="s">
+        <v>558</v>
+      </c>
+      <c r="E38" s="8" t="s">
+        <v>703</v>
+      </c>
+      <c r="F38" s="8" t="s">
+        <v>704</v>
+      </c>
+      <c r="G38" s="8" t="s">
+        <v>705</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" ht="166.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="4" t="s">
+        <v>556</v>
+      </c>
+      <c r="B39" s="8" t="s">
+        <v>706</v>
+      </c>
+      <c r="C39" s="6">
+        <v>41076</v>
+      </c>
+      <c r="D39" s="4" t="s">
+        <v>558</v>
+      </c>
+      <c r="E39" s="8" t="s">
+        <v>707</v>
+      </c>
+      <c r="F39" s="8" t="s">
+        <v>708</v>
+      </c>
+      <c r="G39" s="8" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" ht="144" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="4" t="s">
+        <v>556</v>
+      </c>
+      <c r="B40" s="8" t="s">
+        <v>710</v>
+      </c>
+      <c r="C40" s="6">
+        <v>41077</v>
+      </c>
+      <c r="D40" s="4" t="s">
+        <v>558</v>
+      </c>
+      <c r="E40" s="8" t="s">
+        <v>711</v>
+      </c>
+      <c r="F40" s="8" t="s">
+        <v>712</v>
+      </c>
+      <c r="G40" s="8" t="s">
+        <v>713</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="4" t="s">
+        <v>556</v>
+      </c>
+      <c r="B41" s="4" t="s">
+        <v>715</v>
+      </c>
+      <c r="C41" s="6">
+        <v>41079</v>
+      </c>
+      <c r="D41" s="4" t="s">
+        <v>558</v>
+      </c>
+      <c r="E41" s="8" t="s">
+        <v>714</v>
+      </c>
+      <c r="F41" s="8" t="s">
+        <v>716</v>
+      </c>
+      <c r="G41" s="8" t="s">
+        <v>717</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" ht="117.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="4" t="s">
+        <v>556</v>
+      </c>
+      <c r="B42" s="4" t="s">
+        <v>718</v>
+      </c>
+      <c r="C42" s="6">
+        <v>41080</v>
+      </c>
+      <c r="D42" s="4" t="s">
+        <v>558</v>
+      </c>
+      <c r="E42" s="8" t="s">
+        <v>719</v>
+      </c>
+      <c r="F42" s="8" t="s">
+        <v>720</v>
+      </c>
+      <c r="G42" s="8" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" ht="155.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="4" t="s">
+        <v>556</v>
+      </c>
+      <c r="B43" s="8" t="s">
+        <v>723</v>
+      </c>
+      <c r="C43" s="6">
+        <v>41081</v>
+      </c>
+      <c r="D43" s="4" t="s">
+        <v>558</v>
+      </c>
+      <c r="E43" s="8" t="s">
+        <v>722</v>
+      </c>
+      <c r="F43" s="8" t="s">
+        <v>724</v>
+      </c>
+      <c r="G43" s="8" t="s">
+        <v>725</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" ht="166.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="4" t="s">
+        <v>556</v>
+      </c>
+      <c r="B44" s="8" t="s">
+        <v>726</v>
+      </c>
+      <c r="C44" s="6">
+        <v>41082</v>
+      </c>
+      <c r="D44" s="4" t="s">
+        <v>558</v>
+      </c>
+      <c r="E44" s="8" t="s">
+        <v>727</v>
+      </c>
+      <c r="F44" s="8" t="s">
+        <v>728</v>
+      </c>
+      <c r="G44" s="8" t="s">
+        <v>729</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" ht="210.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="4" t="s">
+        <v>556</v>
+      </c>
+      <c r="B45" s="18" t="s">
+        <v>730</v>
+      </c>
+      <c r="C45" s="6">
+        <v>41083</v>
+      </c>
+      <c r="D45" s="4" t="s">
+        <v>558</v>
+      </c>
+      <c r="E45" s="8" t="s">
+        <v>731</v>
+      </c>
+      <c r="F45" s="8" t="s">
+        <v>732</v>
+      </c>
+      <c r="G45" s="8" t="s">
+        <v>733</v>
+      </c>
     </row>
     <row r="46" spans="1:7" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="1"/>
-      <c r="B46" s="1"/>
-      <c r="C46" s="1"/>
-      <c r="D46" s="1"/>
-      <c r="E46" s="1"/>
-      <c r="F46" s="1"/>
-      <c r="G46" s="1"/>
+      <c r="A46" s="4"/>
+      <c r="B46" s="4"/>
+      <c r="C46" s="4"/>
+      <c r="D46" s="4"/>
+      <c r="E46" s="4"/>
+      <c r="F46" s="4"/>
+      <c r="G46" s="4"/>
     </row>
     <row r="47" spans="1:7" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="1"/>
-      <c r="B47" s="1"/>
-      <c r="C47" s="1"/>
-      <c r="D47" s="1"/>
-      <c r="E47" s="1"/>
-      <c r="F47" s="1"/>
-      <c r="G47" s="1"/>
+      <c r="A47" s="4"/>
+      <c r="B47" s="4"/>
+      <c r="C47" s="4"/>
+      <c r="D47" s="4"/>
+      <c r="E47" s="4"/>
+      <c r="F47" s="4"/>
+      <c r="G47" s="4"/>
     </row>
     <row r="48" spans="1:7" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="1"/>
-      <c r="B48" s="1"/>
-      <c r="C48" s="1"/>
-      <c r="D48" s="1"/>
-      <c r="E48" s="1"/>
-      <c r="F48" s="1"/>
-      <c r="G48" s="1"/>
+      <c r="A48" s="4"/>
+      <c r="B48" s="4"/>
+      <c r="C48" s="4"/>
+      <c r="D48" s="4"/>
+      <c r="E48" s="4"/>
+      <c r="F48" s="4"/>
+      <c r="G48" s="4"/>
     </row>
     <row r="49" spans="1:7" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="1"/>
-      <c r="B49" s="1"/>
-      <c r="C49" s="1"/>
-      <c r="D49" s="1"/>
-      <c r="E49" s="1"/>
-      <c r="F49" s="1"/>
-      <c r="G49" s="1"/>
+      <c r="A49" s="4"/>
+      <c r="B49" s="4"/>
+      <c r="C49" s="4"/>
+      <c r="D49" s="4"/>
+      <c r="E49" s="4"/>
+      <c r="F49" s="4"/>
+      <c r="G49" s="4"/>
     </row>
     <row r="50" spans="1:7" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="1"/>
-      <c r="B50" s="1"/>
-      <c r="C50" s="1"/>
-      <c r="D50" s="1"/>
-      <c r="E50" s="1"/>
-      <c r="F50" s="1"/>
-      <c r="G50" s="1"/>
+      <c r="A50" s="4"/>
+      <c r="B50" s="4"/>
+      <c r="C50" s="4"/>
+      <c r="D50" s="4"/>
+      <c r="E50" s="4"/>
+      <c r="F50" s="4"/>
+      <c r="G50" s="4"/>
     </row>
     <row r="51" spans="1:7" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="1"/>
-      <c r="B51" s="1"/>
-      <c r="C51" s="1"/>
-      <c r="D51" s="1"/>
-      <c r="E51" s="1"/>
-      <c r="F51" s="1"/>
-      <c r="G51" s="1"/>
+      <c r="A51" s="4"/>
+      <c r="B51" s="4"/>
+      <c r="C51" s="4"/>
+      <c r="D51" s="4"/>
+      <c r="E51" s="4"/>
+      <c r="F51" s="4"/>
+      <c r="G51" s="4"/>
     </row>
     <row r="52" spans="1:7" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="1"/>
-      <c r="B52" s="1"/>
-      <c r="C52" s="1"/>
-      <c r="D52" s="1"/>
-      <c r="E52" s="1"/>
-      <c r="F52" s="1"/>
-      <c r="G52" s="1"/>
+      <c r="A52" s="4"/>
+      <c r="B52" s="4"/>
+      <c r="C52" s="4"/>
+      <c r="D52" s="4"/>
+      <c r="E52" s="4"/>
+      <c r="F52" s="4"/>
+      <c r="G52" s="4"/>
     </row>
     <row r="53" spans="1:7" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="1"/>

</xml_diff>

<commit_message>
ultimos cambios en la tesis
</commit_message>
<xml_diff>
--- a/Cuadro de noticias.xlsx
+++ b/Cuadro de noticias.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{001DB303-9B90-47AA-854A-FFB74D960E0A}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5258031F-3900-4EE0-B6CF-FC097627BE82}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Ultima Hora" sheetId="1" r:id="rId1"/>
@@ -2707,8 +2707,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:G172"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G87" sqref="G87"/>
+    <sheetView tabSelected="1" topLeftCell="A102" workbookViewId="0">
+      <selection activeCell="G102" sqref="G102"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3248,7 +3248,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" ht="54.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
         <v>6</v>
       </c>
@@ -6200,8 +6200,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:G65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+    <sheetView topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
cambios en el cuaderno
</commit_message>
<xml_diff>
--- a/Cuadro de noticias.xlsx
+++ b/Cuadro de noticias.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5258031F-3900-4EE0-B6CF-FC097627BE82}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2F5C7DF-B5BE-4642-A713-CFD023BA040F}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2400,14 +2400,14 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -2707,8 +2707,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:G172"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A102" workbookViewId="0">
-      <selection activeCell="G102" sqref="G102"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
ultimos cambios en el cuaderno
</commit_message>
<xml_diff>
--- a/Cuadro de noticias.xlsx
+++ b/Cuadro de noticias.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21231"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Documents\TESIS\Tesis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F18171F-71FB-4FF1-BE1E-86442098FCCC}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160"/>
   </bookViews>
   <sheets>
     <sheet name="Ultima Hora" sheetId="1" r:id="rId1"/>
@@ -2272,7 +2271,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -2704,11 +2703,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:G172"/>
   <sheetViews>
-    <sheetView topLeftCell="A116" workbookViewId="0">
-      <selection activeCell="B117" sqref="B117"/>
+    <sheetView tabSelected="1" topLeftCell="A57" workbookViewId="0">
+      <selection activeCell="B59" sqref="B59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3432,7 +3431,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="33" spans="1:7" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" ht="66.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="4" t="s">
         <v>6</v>
       </c>
@@ -3524,7 +3523,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="37" spans="1:7" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7" ht="66.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="4" t="s">
         <v>6</v>
       </c>
@@ -3547,7 +3546,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="38" spans="1:7" ht="79.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="4" t="s">
         <v>6</v>
       </c>
@@ -3616,7 +3615,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="41" spans="1:7" ht="173.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:7" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="4" t="s">
         <v>6</v>
       </c>
@@ -3800,7 +3799,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="49" spans="1:7" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:7" ht="51" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="4" t="s">
         <v>6</v>
       </c>
@@ -3823,7 +3822,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="50" spans="1:7" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:7" ht="67.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="4" t="s">
         <v>6</v>
       </c>
@@ -4030,7 +4029,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="59" spans="1:7" ht="91.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:7" ht="90.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="4" t="s">
         <v>6</v>
       </c>
@@ -6197,11 +6196,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>